<commit_message>
fsk_distance_measure_demo2: serial rev test ok
</commit_message>
<xml_diff>
--- a/embedded/fsk_distance_measure_demo2/DOC/pin分配.xlsx
+++ b/embedded/fsk_distance_measure_demo2/DOC/pin分配.xlsx
@@ -14,11 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
-  <si>
-    <t xml:space="preserve"> 序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>PIN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,10 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用途</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>临时功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -124,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FSK控制输出,TIMERA_CH2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PB5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -152,15 +140,80 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结果输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM6_1_PWMA
+TIMA_1_PWM1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM6_1_PWMB 
+TIMA_1_PWM5 
+TIMA_3_PWM2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIMA_2_PWM1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可使用的用途</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIMA_3_PWM5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIMA_4_PWM1
+TIMA_6_PWM8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIMA_3_PWM2
+TIMA_6_PWM7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK控制输出,TIMERA3_CH2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按用户要求输出,TIMA_1_PWM1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -222,7 +275,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -234,6 +287,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -546,32 +602,32 @@
     <col min="2" max="3" width="13.73046875" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.19921875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.06640625" style="2"/>
-    <col min="6" max="6" width="10.265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -579,50 +635,54 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="27">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="27">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
@@ -630,13 +690,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -647,13 +707,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -664,13 +724,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3"/>
@@ -681,13 +741,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="3"/>
@@ -698,13 +758,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -715,36 +775,89 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="27">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="40.5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>